<commit_message>
Updating Data S on website
</commit_message>
<xml_diff>
--- a/Website/tropics/supplementary-data/forest_cover_change_uncertainty.xlsx
+++ b/Website/tropics/supplementary-data/forest_cover_change_uncertainty.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -1077,8 +1077,8 @@
   </sheetPr>
   <dimension ref="A1:W358"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A310" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="W248" activeCellId="0" sqref="W248"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>